<commit_message>
Actualización scripts DDMRP y manual de usuario
</commit_message>
<xml_diff>
--- a/Resumen_Consumo_LT_VentanaFija.xlsx
+++ b/Resumen_Consumo_LT_VentanaFija.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trimarinegroup.sharepoint.com/sites/SUPPLYCHAINGRALCO/Documentos compartidos/2024/POWER BI 2024/Almacen_PBI/RAW/PROYECTO MATERIAL POINT REVIEW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_612FDDA6ECB50FC04D4FA106D278361C00FFE8FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CF688B-1BB6-434A-84AE-77FF22008F4C}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_612FDDA6ECB50FC04D4FA106D278361C00FFE8FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92F34CAB-8721-4A2C-AC1C-19EF1929EF98}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$157</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1035,7 +1038,7 @@
   <dimension ref="A1:L157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7020,17 +7023,23 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L157" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L157">
+    <sortCondition descending="1" ref="L2:L157"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f289a69-df02-44c5-87d6-7d65c15e90e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0f127205-4eb4-42c3-87dd-12c53b247890" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7275,20 +7284,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f289a69-df02-44c5-87d6-7d65c15e90e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0f127205-4eb4-42c3-87dd-12c53b247890" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350CEAAA-605A-44EA-B4E3-20001D29DC0D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42149FB-CA2B-4653-91CD-E16A06B68705}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f289a69-df02-44c5-87d6-7d65c15e90e3"/>
+    <ds:schemaRef ds:uri="0f127205-4eb4-42c3-87dd-12c53b247890"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7313,12 +7323,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42149FB-CA2B-4653-91CD-E16A06B68705}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350CEAAA-605A-44EA-B4E3-20001D29DC0D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f289a69-df02-44c5-87d6-7d65c15e90e3"/>
-    <ds:schemaRef ds:uri="0f127205-4eb4-42c3-87dd-12c53b247890"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>